<commit_message>
cv updates and multiple description bullets
</commit_message>
<xml_diff>
--- a/cv_data.xlsx
+++ b/cv_data.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="147">
   <si>
     <t>section</t>
   </si>
@@ -37,6 +37,12 @@
     <t>description</t>
   </si>
   <si>
+    <t>desc1</t>
+  </si>
+  <si>
+    <t>desc2</t>
+  </si>
+  <si>
     <t>in_resume</t>
   </si>
   <si>
@@ -199,7 +205,7 @@
     <t xml:space="preserve">Assist Dr. Andreas Handel in research for the Center for Influenza Vaccine Research for High-Risk Populations (CIVR-HRP) grant at the University of Georgia. Aid in research and data analysis on influenza vaccines, particularly data related to universal influenza vaccine development. </t>
   </si>
   <si>
-    <t>SWEP Volunteer</t>
+    <t>Research Assistant</t>
   </si>
   <si>
     <t>Atlanta, GA</t>
@@ -208,7 +214,10 @@
     <t>Centers for Disease Control and Prevention, National Center on Birth Defects and Developmental Disabilities</t>
   </si>
   <si>
-    <t xml:space="preserve">Review and analyze incoming data as a member of the MAT-LINK surveillance team (MAT-LINK: MATernaL and Infant NetworK to Understand Outcomes Associated with Medication for Opioid Use Disorder during Pregnancy). Data review includes examination and basic analysis of incoming data from clinical sites, writing and compiling of feedback related to data quality, and assessing data for potential analyses and research projects. Participate in data and analysis meetings and collaborate with team members on research and analysis plans. </t>
+    <t xml:space="preserve">In support of the MAT-LINK (MATernaL and Infant NetworK to Understand Outcomes Associated with Medication for Opioid Use Disorder during Pregnancy) team, fulfill the following duties and responsibilities: </t>
+  </si>
+  <si>
+    <t>Conduct data cleaning, analysis, and management using statistical software (e.g. SAS, R, etc.), and interpretation. Support team on data quality assurance checks, and other reviews of data. Conduct literature reviews related to opioid use disorder, pregnancy, and other topics. Develop instructional material on use of R and RMarkdown for reports and publications. Support the development of statistical briefs, standard operating procedures, and publically available code for outcome identification using ICD-9 and ICD-10 codes. Perform primary and secondary analyses for manuscript development.</t>
   </si>
   <si>
     <t>Graduate Departmental Assisant</t>
@@ -271,9 +280,6 @@
     <t>Secretary</t>
   </si>
   <si>
-    <t>University of Georgia College of Public Health</t>
-  </si>
-  <si>
     <t>Graduate Scholars of Epidemiology &amp; Biostatistics (GSEB)</t>
   </si>
   <si>
@@ -283,6 +289,18 @@
     <t>Managed fundraising events and community food pantry. Planned and recorded regular executive board and general body meetings. Developed and led events open to department and college students. Maintained communication with department members to assess student needs and announce organization events. Maintained records for future executive board members.</t>
   </si>
   <si>
+    <t>Student Representative</t>
+  </si>
+  <si>
+    <t>College of Public Health Curriculum Committee</t>
+  </si>
+  <si>
+    <t>2022-2023</t>
+  </si>
+  <si>
+    <t>Review, inform changes, and vote on new College of Public Health degrees, certificates, and classes.</t>
+  </si>
+  <si>
     <t>org</t>
   </si>
   <si>
@@ -299,6 +317,27 @@
   </si>
   <si>
     <t>Council of State and Territorial Epidemiologists (CSTE)</t>
+  </si>
+  <si>
+    <t>presentations</t>
+  </si>
+  <si>
+    <t>Challenge Study Ethics</t>
+  </si>
+  <si>
+    <t>Infectious Disease Interest Group</t>
+  </si>
+  <si>
+    <t>In collaboration with a colleague, developed and led a presentation on the background and basics of challenge studies (or, controlled human infection studies) and led a group discussion on ethical concerns and considerations in the studies themselves and whether data from unethical studies should be used as secondary analyses and publications.</t>
+  </si>
+  <si>
+    <t>Dengue Case-Control Study Review and Critique</t>
+  </si>
+  <si>
+    <t>Case-Control Design, Implemetation, and Analysis</t>
+  </si>
+  <si>
+    <t>Presented and critiqued "Risk factors of dengue fever in an urban area in Vietnam: a case-control study” by Nguyen-Tien et al. (2021) study design, methods, and analysis for epidemiology PhD case-control methods course.</t>
   </si>
   <si>
     <t>Name of language</t>
@@ -593,7 +632,7 @@
     <col customWidth="1" min="5" max="5" width="10.0"/>
     <col customWidth="1" min="6" max="6" width="9.63"/>
     <col customWidth="1" min="7" max="7" width="29.13"/>
-    <col customWidth="1" min="8" max="8" width="16.25"/>
+    <col customWidth="1" min="8" max="10" width="16.25"/>
   </cols>
   <sheetData>
     <row r="1" ht="18.75" customHeight="1">
@@ -621,8 +660,12 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
@@ -637,43 +680,47 @@
       <c r="V1" s="3"/>
       <c r="W1" s="3"/>
       <c r="X1" s="3"/>
+      <c r="Y1" s="3"/>
+      <c r="Z1" s="3"/>
     </row>
     <row r="2">
       <c r="A2" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E2" s="4">
         <v>2022.0</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="6"/>
-      <c r="H2" s="4" t="b">
+      <c r="H2" s="4"/>
+      <c r="I2" s="4"/>
+      <c r="J2" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>11</v>
       </c>
       <c r="E3" s="4">
         <v>2020.0</v>
@@ -682,22 +729,24 @@
         <v>2022.0</v>
       </c>
       <c r="G3" s="6"/>
-      <c r="H3" s="4" t="b">
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="E4" s="4">
         <v>2018.0</v>
@@ -706,22 +755,24 @@
         <v>2020.0</v>
       </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="4" t="b">
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="4">
         <v>2014.0</v>
@@ -730,74 +781,80 @@
         <v>2015.0</v>
       </c>
       <c r="G5" s="7"/>
-      <c r="H5" s="4" t="b">
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E7" s="4">
         <v>2021.0</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="4" t="b">
+        <v>26</v>
+      </c>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E8" s="4">
         <v>2022.0</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H8" s="4" t="b">
+        <v>28</v>
+      </c>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E9" s="4">
         <v>2021.0</v>
@@ -806,24 +863,26 @@
         <v>2022.0</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H9" s="4" t="b">
-        <v>1</v>
+        <v>30</v>
+      </c>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="E10" s="4">
         <v>2021.0</v>
@@ -832,21 +891,23 @@
         <v>2022.0</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" s="4" t="b">
-        <v>1</v>
+        <v>32</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -854,19 +915,21 @@
         <v>2021.0</v>
       </c>
       <c r="G11" s="5"/>
-      <c r="H11" s="4" t="b">
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
@@ -874,19 +937,21 @@
         <v>2020.0</v>
       </c>
       <c r="G12" s="5"/>
-      <c r="H12" s="4" t="b">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
@@ -894,19 +959,21 @@
         <v>2020.0</v>
       </c>
       <c r="G13" s="5"/>
-      <c r="H13" s="4" t="b">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
@@ -914,19 +981,21 @@
         <v>2019.0</v>
       </c>
       <c r="G14" s="5"/>
-      <c r="H14" s="4" t="b">
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
@@ -934,218 +1003,242 @@
         <v>2019.0</v>
       </c>
       <c r="G15" s="5"/>
-      <c r="H15" s="4" t="b">
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
       <c r="G16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="H16" s="4" t="b">
+        <v>44</v>
+      </c>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="4" t="b">
+        <v>46</v>
+      </c>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
       <c r="G18" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="H18" s="4" t="b">
+        <v>48</v>
+      </c>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="4"/>
       <c r="E19" s="4"/>
       <c r="F19" s="4"/>
       <c r="G19" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="H19" s="4" t="b">
+        <v>50</v>
+      </c>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
       <c r="F20" s="4"/>
       <c r="G20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="H20" s="4" t="b">
+        <v>52</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
       <c r="G21" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="H21" s="4" t="b">
+        <v>54</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
       <c r="G22" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="4" t="b">
+        <v>56</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
       <c r="G23" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="H23" s="4" t="b">
+        <v>58</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E24" s="4">
         <v>2022.0</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="H24" s="4" t="b">
+        <v>62</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="E25" s="4">
         <v>2022.0</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="H25" s="4" t="b">
-        <v>0</v>
+        <v>66</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="E26" s="4">
         <v>2021.0</v>
@@ -1154,24 +1247,26 @@
         <v>2022.0</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H26" s="4" t="b">
+        <v>69</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="E27" s="4">
         <v>2018.0</v>
@@ -1180,24 +1275,26 @@
         <v>2019.0</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="H27" s="4" t="b">
+        <v>72</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="E28" s="4">
         <v>2016.0</v>
@@ -1206,24 +1303,26 @@
         <v>2016.0</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="H28" s="4" t="b">
+        <v>76</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="E29" s="4">
         <v>2016.0</v>
@@ -1232,27 +1331,31 @@
         <v>2016.0</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="4" t="b">
+        <v>79</v>
+      </c>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C30" s="5"/>
       <c r="D30" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
       <c r="G30" s="5"/>
       <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
     </row>
     <row r="31">
       <c r="A31" s="4"/>
@@ -1263,50 +1366,79 @@
       <c r="F31" s="4"/>
       <c r="G31" s="5"/>
       <c r="H31" s="4"/>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
     </row>
     <row r="32">
       <c r="A32" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H32" s="4" t="b">
+        <v>86</v>
+      </c>
+      <c r="H32" s="4"/>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="4" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>85</v>
+        <v>13</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="H33" s="4" t="b">
+        <v>90</v>
+      </c>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J34" s="4" t="b">
         <v>1</v>
       </c>
     </row>
@@ -1319,59 +1451,65 @@
       <c r="F35" s="4"/>
       <c r="G35" s="5"/>
       <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36">
       <c r="A36" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="E36" s="4">
         <v>2021.0</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H36" s="4" t="b">
+        <v>25</v>
+      </c>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C37" s="5"/>
       <c r="D37" s="4" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E37" s="4">
         <v>2021.0</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G37" s="5"/>
-      <c r="H37" s="4" t="b">
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C38" s="5"/>
       <c r="D38" s="4" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="E38" s="4">
         <v>2019.0</v>
@@ -1380,75 +1518,110 @@
         <v>2020.0</v>
       </c>
       <c r="G38" s="5"/>
-      <c r="H38" s="4" t="b">
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="E39" s="4">
         <v>2019.0</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G39" s="5"/>
-      <c r="H39" s="4" t="b">
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="4" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C40" s="5"/>
       <c r="D40" s="4" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E40" s="4">
         <v>2021.0</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G40" s="5"/>
-      <c r="H40" s="4" t="b">
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="41">
-      <c r="A41" s="4"/>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="5"/>
+      <c r="A41" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B41" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>104</v>
+      </c>
       <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="42">
-      <c r="A42" s="4"/>
-      <c r="B42" s="5"/>
-      <c r="C42" s="5"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="5"/>
+      <c r="A42" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2022.0</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>107</v>
+      </c>
       <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4" t="b">
+        <v>1</v>
+      </c>
     </row>
     <row r="43">
-      <c r="A43" s="4"/>
       <c r="B43" s="5"/>
       <c r="C43" s="5"/>
       <c r="D43" s="4"/>
@@ -1456,6 +1629,8 @@
       <c r="F43" s="4"/>
       <c r="G43" s="5"/>
       <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
     </row>
     <row r="44">
       <c r="A44" s="4"/>
@@ -1466,6 +1641,8 @@
       <c r="F44" s="4"/>
       <c r="G44" s="5"/>
       <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
     </row>
     <row r="45">
       <c r="A45" s="4"/>
@@ -1476,6 +1653,8 @@
       <c r="F45" s="4"/>
       <c r="G45" s="5"/>
       <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
     </row>
     <row r="46">
       <c r="A46" s="4"/>
@@ -1486,6 +1665,8 @@
       <c r="F46" s="4"/>
       <c r="G46" s="5"/>
       <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
     </row>
     <row r="47">
       <c r="B47" s="5"/>
@@ -6493,10 +6674,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="11" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -6525,10 +6706,10 @@
     </row>
     <row r="2">
       <c r="A2" s="13" t="s">
-        <v>97</v>
+        <v>110</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -6557,7 +6738,7 @@
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B3" s="4">
         <v>5.0</v>
@@ -6565,7 +6746,7 @@
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="B4" s="4">
         <v>4.5</v>
@@ -6573,7 +6754,7 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="B5" s="4">
         <v>4.0</v>
@@ -6581,7 +6762,7 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B6" s="4">
         <v>4.0</v>
@@ -6589,7 +6770,7 @@
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="B7" s="4">
         <v>3.5</v>
@@ -6597,7 +6778,7 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="B8" s="4">
         <v>3.0</v>
@@ -6605,7 +6786,7 @@
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B9" s="4">
         <v>3.0</v>
@@ -6632,10 +6813,10 @@
   <sheetData>
     <row r="1" ht="33.0" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C1" s="16"/>
       <c r="D1" s="16"/>
@@ -6667,7 +6848,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="17" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
@@ -6696,34 +6877,34 @@
     </row>
     <row r="3">
       <c r="A3" s="18" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7">
@@ -9732,13 +9913,13 @@
   <sheetData>
     <row r="1" ht="36.75" customHeight="1">
       <c r="A1" s="15" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D1" s="16"/>
       <c r="E1" s="16"/>
@@ -9770,65 +9951,65 @@
         <v>2</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="4" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>

</xml_diff>